<commit_message>
Update with Kirchoff's Quiz
</commit_message>
<xml_diff>
--- a/Data/TechData.xlsx
+++ b/Data/TechData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17700"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="2" r:id="rId1"/>
@@ -706,8 +706,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,7 +998,7 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,7 +1206,7 @@
   <dimension ref="A1:R3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1358,7 +1358,7 @@
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1775,8 +1775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2055,7 +2055,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>